<commit_message>
Resolved errors and added testng xml files for every test classes
</commit_message>
<xml_diff>
--- a/src/resources/testdata/ForgotPasswordTestdata.xlsx
+++ b/src/resources/testdata/ForgotPasswordTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99A0037-D109-4E94-9EA6-101F2DF94B03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38226B87-C6B6-43D1-BB9F-3DC440F7669D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{28C51002-70FA-4C32-AECD-F59725DEA7A7}"/>
   </bookViews>
@@ -49,15 +49,6 @@
     <t>confirmpass</t>
   </si>
   <si>
-    <t>fake@g.com</t>
-  </si>
-  <si>
-    <t>fake@12345</t>
-  </si>
-  <si>
-    <t>fake10@g.com</t>
-  </si>
-  <si>
     <t>wk@g.com</t>
   </si>
   <si>
@@ -68,6 +59,15 @@
   </si>
   <si>
     <t>sk@12345</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>anuj.lpu1@gmail.com</t>
+  </si>
+  <si>
+    <t>wk@1234</t>
   </si>
 </sst>
 </file>
@@ -448,10 +448,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -469,30 +472,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>4567321231</v>
+        <v>9009857868</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -500,6 +503,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{14FB134D-A0F5-46E8-BDDA-F8DC6BD8595A}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{3508AEFB-4CBD-4051-ABAF-4B5F68541398}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{B4DD0E70-807F-474E-A4C7-97FD9922A577}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{03FA842B-37B3-4CDA-9735-3BE73AF26CA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -510,10 +514,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -531,30 +538,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>